<commit_message>
Testing github action (xlsx)
</commit_message>
<xml_diff>
--- a/PythonCSharpener/localization_tool/CoPick.Logging.xlsx
+++ b/PythonCSharpener/localization_tool/CoPick.Logging.xlsx
@@ -99,14 +99,71 @@
     <t>Invalid log path! Log files could not be written.</t>
   </si>
   <si>
-    <t>로그 경로가 유효하지 않습니다.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로그</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>경로가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>유효합니다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +196,13 @@
       <color rgb="FF1D1C1D"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -459,7 +523,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD1048576"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -571,6 +635,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Testing github action ( xlsx localization value change )
</commit_message>
<xml_diff>
--- a/PythonCSharpener/localization_tool/CoPick.Logging.xlsx
+++ b/PythonCSharpener/localization_tool/CoPick.Logging.xlsx
@@ -104,7 +104,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>로그</t>
+      <t>캡쳐</t>
     </r>
     <r>
       <rPr>
@@ -123,7 +123,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>경로가</t>
+      <t>가능</t>
     </r>
     <r>
       <rPr>
@@ -142,7 +142,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>유효하지</t>
+      <t>영역이</t>
     </r>
     <r>
       <rPr>
@@ -161,7 +161,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>않습니다</t>
+      <t>없습니다</t>
     </r>
     <r>
       <rPr>
@@ -183,7 +183,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>캡쳐</t>
+      <t>로그</t>
     </r>
     <r>
       <rPr>
@@ -202,7 +202,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>가능</t>
+      <t>경로가</t>
     </r>
     <r>
       <rPr>
@@ -221,7 +221,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>영역이</t>
+      <t>유효하지</t>
     </r>
     <r>
       <rPr>
@@ -240,7 +240,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>없습니다</t>
+      <t>않습니까</t>
     </r>
     <r>
       <rPr>
@@ -249,7 +249,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>.</t>
+      <t>?</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -713,7 +713,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -724,7 +724,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing github action ( cs token , xlsx value )
</commit_message>
<xml_diff>
--- a/PythonCSharpener/localization_tool/CoPick.Logging.xlsx
+++ b/PythonCSharpener/localization_tool/CoPick.Logging.xlsx
@@ -104,6 +104,114 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
+      <t>로그</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>경로가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>유효하지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>않습니다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>번역값이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>달라지면</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
       <t>캡쳐</t>
     </r>
     <r>
@@ -170,77 +278,93 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>.</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>로그</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>경로가</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>유효하지</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>않습니까</t>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>달라진</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> xlsx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>와</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>같이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>코드</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>올리면</t>
     </r>
     <r>
       <rPr>
@@ -618,7 +742,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -713,7 +837,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -724,7 +848,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>